<commit_message>
update close broser, profile page and add feedback
</commit_message>
<xml_diff>
--- a/Data/Matching+value.xlsx
+++ b/Data/Matching+value.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -220,13 +220,16 @@
   </si>
   <si>
     <t>Indyfin outlook</t>
+  </si>
+  <si>
+    <t>Retirement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,12 +242,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF1B1B1B"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="9"/>
@@ -349,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -360,7 +357,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -368,9 +365,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -380,16 +374,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -696,69 +690,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="8" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="35.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -766,8 +760,8 @@
       <c r="A2" s="2">
         <v>1001</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>15</v>
+      <c r="B2" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>19</v>
@@ -781,7 +775,7 @@
       <c r="F2" s="3">
         <v>78539</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -790,7 +784,7 @@
       <c r="I2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>53</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -834,7 +828,7 @@
       <c r="I3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>52</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -854,7 +848,7 @@
       <c r="A4" s="2">
         <v>1003</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -869,7 +863,7 @@
       <c r="F4">
         <v>67001</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -878,13 +872,13 @@
       <c r="I4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>54</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>67</v>
       </c>
       <c r="M4" s="6" t="s">
@@ -895,10 +889,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>1004</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -913,7 +907,7 @@
       <c r="F5">
         <v>99501</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -922,27 +916,27 @@
       <c r="I5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>28</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>1005</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -957,7 +951,7 @@
       <c r="F6">
         <v>48005</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -966,27 +960,27 @@
       <c r="I6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>56</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>62</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>1006</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1001,7 +995,7 @@
       <c r="F7">
         <v>85001</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1010,19 +1004,19 @@
       <c r="I7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="8" t="s">
         <v>57</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="15" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>